<commit_message>
code updates and minor tweaks
</commit_message>
<xml_diff>
--- a/input_data/flow_scen/FallFlows20250819_Draft 1.xlsx
+++ b/input_data/flow_scen/FallFlows20250819_Draft 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29203"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/ebuttermore_usbr_gov/Documents/Desktop/SRG/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/cehlo_usbr_gov/Documents/Redd_dewatering/Fall_Flow_Redd_Dewatering/input_data/flow_scen/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{086A6FC7-FD32-4CF8-BA3A-50FE3EF49E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4695" yWindow="615" windowWidth="23235" windowHeight="14265" tabRatio="876" xr2:uid="{8B6B0201-DD1B-4D0A-8FA2-1793C828B1EC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="876" xr2:uid="{8B6B0201-DD1B-4D0A-8FA2-1793C828B1EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Keswick Flow Alternatives" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Keswick Flow Chart Fall only" sheetId="12" r:id="rId5"/>
     <sheet name="Scenario Description" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -329,7 +329,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -7763,16 +7763,16 @@
                   <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>10000000</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>10000000</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>10000000</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>10000000</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>10000000</c:v>
@@ -8531,7 +8531,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -8539,6 +8538,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -9385,16 +9385,16 @@
                   <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>10000000</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>10000000</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>10000000</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>10000000</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>10000000</c:v>
@@ -24209,7 +24209,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -24217,6 +24216,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -25362,7 +25362,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{B9A0DFFB-0EAB-4130-A4A2-055D67D97DCF}">
   <sheetPr/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="104" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -25450,7 +25450,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8667750" cy="6296025"/>
+    <xdr:ext cx="8673245" cy="6291995"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -25513,9 +25513,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -25553,7 +25553,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -25659,7 +25659,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -25801,7 +25801,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -25812,13 +25812,13 @@
   <dimension ref="A1:Q245"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="M96" sqref="M96"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C218" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="A233" sqref="A233"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.42578125" style="18" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" style="18" customWidth="1"/>
@@ -25835,13 +25835,13 @@
     <col min="18" max="16384" width="8.5703125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75">
+    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="26"/>
     </row>
-    <row r="2" spans="1:17" s="27" customFormat="1">
+    <row r="2" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>1</v>
       </c>
@@ -25888,7 +25888,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="27" customFormat="1">
+    <row r="3" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="38">
         <v>45870</v>
       </c>
@@ -25933,7 +25933,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="27" customFormat="1">
+    <row r="4" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="38">
         <v>45871</v>
       </c>
@@ -25978,7 +25978,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="27" customFormat="1">
+    <row r="5" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="38">
         <v>45872</v>
       </c>
@@ -26023,7 +26023,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="27" customFormat="1">
+    <row r="6" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="38">
         <v>45873</v>
       </c>
@@ -26068,7 +26068,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="27" customFormat="1">
+    <row r="7" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="38">
         <v>45874</v>
       </c>
@@ -26113,7 +26113,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="27" customFormat="1">
+    <row r="8" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="38">
         <v>45875</v>
       </c>
@@ -26158,7 +26158,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="27" customFormat="1">
+    <row r="9" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="38">
         <v>45876</v>
       </c>
@@ -26203,7 +26203,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="27" customFormat="1">
+    <row r="10" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="38">
         <v>45877</v>
       </c>
@@ -26248,7 +26248,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="27" customFormat="1">
+    <row r="11" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="38">
         <v>45878</v>
       </c>
@@ -26293,7 +26293,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="27" customFormat="1">
+    <row r="12" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="38">
         <v>45879</v>
       </c>
@@ -26338,7 +26338,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="27" customFormat="1">
+    <row r="13" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="38">
         <v>45880</v>
       </c>
@@ -26383,7 +26383,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="27" customFormat="1">
+    <row r="14" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="38">
         <v>45881</v>
       </c>
@@ -26428,7 +26428,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="27" customFormat="1">
+    <row r="15" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="38">
         <v>45882</v>
       </c>
@@ -26473,7 +26473,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="27" customFormat="1">
+    <row r="16" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="38">
         <v>45883</v>
       </c>
@@ -26518,7 +26518,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="27" customFormat="1">
+    <row r="17" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="38">
         <v>45884</v>
       </c>
@@ -26563,7 +26563,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="27" customFormat="1">
+    <row r="18" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="38">
         <v>45885</v>
       </c>
@@ -26608,7 +26608,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="27" customFormat="1">
+    <row r="19" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="38">
         <v>45886</v>
       </c>
@@ -26653,7 +26653,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="27" customFormat="1">
+    <row r="20" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="38">
         <v>45887</v>
       </c>
@@ -26698,7 +26698,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="21" spans="1:17" s="27" customFormat="1">
+    <row r="21" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="38">
         <v>45888</v>
       </c>
@@ -26743,7 +26743,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="27" customFormat="1">
+    <row r="22" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="38">
         <v>45889</v>
       </c>
@@ -26788,7 +26788,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="27" customFormat="1">
+    <row r="23" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="38">
         <v>45890</v>
       </c>
@@ -26833,7 +26833,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="27" customFormat="1">
+    <row r="24" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="38">
         <v>45891</v>
       </c>
@@ -26875,10 +26875,10 @@
       <c r="P24" s="41"/>
       <c r="Q24" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>10000000</v>
+        <v>-100</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="27" customFormat="1">
+    <row r="25" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="38">
         <v>45892</v>
       </c>
@@ -26920,10 +26920,10 @@
       <c r="P25" s="18"/>
       <c r="Q25" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>10000000</v>
+        <v>-100</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="27" customFormat="1">
+    <row r="26" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="38">
         <v>45893</v>
       </c>
@@ -26965,10 +26965,10 @@
       <c r="P26" s="18"/>
       <c r="Q26" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>10000000</v>
+        <v>-100</v>
       </c>
     </row>
-    <row r="27" spans="1:17" s="27" customFormat="1">
+    <row r="27" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="38">
         <v>45894</v>
       </c>
@@ -27010,10 +27010,10 @@
       <c r="P27" s="18"/>
       <c r="Q27" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>10000000</v>
+        <v>-100</v>
       </c>
     </row>
-    <row r="28" spans="1:17" s="27" customFormat="1">
+    <row r="28" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="38">
         <v>45895</v>
       </c>
@@ -27058,7 +27058,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="27" customFormat="1">
+    <row r="29" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="38">
         <v>45896</v>
       </c>
@@ -27103,7 +27103,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="30" spans="1:17" s="27" customFormat="1">
+    <row r="30" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="38">
         <v>45897</v>
       </c>
@@ -27148,7 +27148,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="27" customFormat="1">
+    <row r="31" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="38">
         <v>45898</v>
       </c>
@@ -27193,7 +27193,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="27" customFormat="1">
+    <row r="32" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="38">
         <v>45899</v>
       </c>
@@ -27238,7 +27238,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="33" spans="1:17" s="27" customFormat="1">
+    <row r="33" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="38">
         <v>45900</v>
       </c>
@@ -27283,7 +27283,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="34" spans="1:17" s="27" customFormat="1">
+    <row r="34" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="38">
         <v>45901</v>
       </c>
@@ -27329,7 +27329,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="27" customFormat="1">
+    <row r="35" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="38">
         <v>45902</v>
       </c>
@@ -27375,7 +27375,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="36" spans="1:17" s="27" customFormat="1">
+    <row r="36" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="38">
         <v>45903</v>
       </c>
@@ -27421,7 +27421,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="27" customFormat="1">
+    <row r="37" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="38">
         <v>45904</v>
       </c>
@@ -27467,7 +27467,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="27" customFormat="1">
+    <row r="38" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="38">
         <v>45905</v>
       </c>
@@ -27513,7 +27513,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="39" spans="1:17">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="38">
         <v>45906</v>
       </c>
@@ -27559,7 +27559,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="40" spans="1:17">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="38">
         <v>45907</v>
       </c>
@@ -27605,7 +27605,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="41" spans="1:17">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="38">
         <v>45908</v>
       </c>
@@ -27651,7 +27651,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="42" spans="1:17">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="38">
         <v>45909</v>
       </c>
@@ -27697,7 +27697,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="43" spans="1:17">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="38">
         <v>45910</v>
       </c>
@@ -27743,7 +27743,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="44" spans="1:17">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="38">
         <v>45911</v>
       </c>
@@ -27789,7 +27789,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="45" spans="1:17">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="38">
         <v>45912</v>
       </c>
@@ -27835,7 +27835,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="46" spans="1:17">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="38">
         <v>45913</v>
       </c>
@@ -27881,7 +27881,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="47" spans="1:17">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="38">
         <v>45914</v>
       </c>
@@ -27927,7 +27927,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="48" spans="1:17">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="38">
         <v>45915</v>
       </c>
@@ -27973,7 +27973,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="49" spans="1:17">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="38">
         <v>45916</v>
       </c>
@@ -28019,7 +28019,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="50" spans="1:17">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="38">
         <v>45917</v>
       </c>
@@ -28065,7 +28065,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="51" spans="1:17">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="38">
         <v>45918</v>
       </c>
@@ -28111,7 +28111,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="52" spans="1:17">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="38">
         <v>45919</v>
       </c>
@@ -28157,7 +28157,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="53" spans="1:17">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="38">
         <v>45920</v>
       </c>
@@ -28203,7 +28203,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="54" spans="1:17">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="38">
         <v>45921</v>
       </c>
@@ -28249,7 +28249,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="55" spans="1:17">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="38">
         <v>45922</v>
       </c>
@@ -28295,7 +28295,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="56" spans="1:17">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="38">
         <v>45923</v>
       </c>
@@ -28341,7 +28341,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="57" spans="1:17">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="38">
         <v>45924</v>
       </c>
@@ -28387,7 +28387,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="58" spans="1:17">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="38">
         <v>45925</v>
       </c>
@@ -28433,7 +28433,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="59" spans="1:17">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="38">
         <v>45926</v>
       </c>
@@ -28479,7 +28479,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="60" spans="1:17">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="38">
         <v>45927</v>
       </c>
@@ -28525,7 +28525,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="61" spans="1:17">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="38">
         <v>45928</v>
       </c>
@@ -28571,7 +28571,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="62" spans="1:17">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="38">
         <v>45929</v>
       </c>
@@ -28617,7 +28617,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="63" spans="1:17">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" s="38">
         <v>45930</v>
       </c>
@@ -28663,7 +28663,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="64" spans="1:17">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" s="38">
         <v>45931</v>
       </c>
@@ -28709,7 +28709,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="65" spans="1:17">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" s="38">
         <v>45932</v>
       </c>
@@ -28755,7 +28755,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="66" spans="1:17">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" s="38">
         <v>45933</v>
       </c>
@@ -28801,7 +28801,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="67" spans="1:17">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" s="38">
         <v>45934</v>
       </c>
@@ -28847,7 +28847,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="68" spans="1:17">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" s="38">
         <v>45935</v>
       </c>
@@ -28893,7 +28893,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="69" spans="1:17">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" s="38">
         <v>45936</v>
       </c>
@@ -28939,7 +28939,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="70" spans="1:17">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" s="38">
         <v>45937</v>
       </c>
@@ -28985,7 +28985,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="71" spans="1:17">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" s="38">
         <v>45938</v>
       </c>
@@ -29031,7 +29031,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="72" spans="1:17">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" s="38">
         <v>45939</v>
       </c>
@@ -29077,7 +29077,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="73" spans="1:17">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" s="38">
         <v>45940</v>
       </c>
@@ -29123,7 +29123,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="74" spans="1:17">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" s="38">
         <v>45941</v>
       </c>
@@ -29169,7 +29169,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="75" spans="1:17">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" s="38">
         <v>45942</v>
       </c>
@@ -29215,7 +29215,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="76" spans="1:17">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" s="38">
         <v>45943</v>
       </c>
@@ -29261,7 +29261,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="77" spans="1:17">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" s="38">
         <v>45944</v>
       </c>
@@ -29307,7 +29307,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="78" spans="1:17">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" s="38">
         <v>45945</v>
       </c>
@@ -29353,7 +29353,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="79" spans="1:17">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" s="38">
         <v>45946</v>
       </c>
@@ -29399,7 +29399,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="80" spans="1:17">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" s="38">
         <v>45947</v>
       </c>
@@ -29445,7 +29445,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="81" spans="1:17">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" s="38">
         <v>45948</v>
       </c>
@@ -29491,7 +29491,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="82" spans="1:17">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" s="38">
         <v>45949</v>
       </c>
@@ -29537,7 +29537,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="83" spans="1:17">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" s="38">
         <v>45950</v>
       </c>
@@ -29583,7 +29583,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="84" spans="1:17">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" s="38">
         <v>45951</v>
       </c>
@@ -29629,7 +29629,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="85" spans="1:17">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85" s="38">
         <v>45952</v>
       </c>
@@ -29675,7 +29675,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="86" spans="1:17">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86" s="38">
         <v>45953</v>
       </c>
@@ -29721,7 +29721,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="87" spans="1:17">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" s="38">
         <v>45954</v>
       </c>
@@ -29767,7 +29767,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="88" spans="1:17">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88" s="38">
         <v>45955</v>
       </c>
@@ -29813,7 +29813,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="89" spans="1:17">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" s="38">
         <v>45956</v>
       </c>
@@ -29859,7 +29859,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="90" spans="1:17">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" s="38">
         <v>45957</v>
       </c>
@@ -29905,7 +29905,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="91" spans="1:17">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91" s="38">
         <v>45958</v>
       </c>
@@ -29951,7 +29951,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="92" spans="1:17">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92" s="38">
         <v>45959</v>
       </c>
@@ -29997,7 +29997,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="93" spans="1:17">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93" s="38">
         <v>45960</v>
       </c>
@@ -30043,7 +30043,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="94" spans="1:17">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94" s="38">
         <v>45961</v>
       </c>
@@ -30089,7 +30089,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="95" spans="1:17">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95" s="38">
         <v>45962</v>
       </c>
@@ -30135,7 +30135,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="96" spans="1:17">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A96" s="38">
         <v>45963</v>
       </c>
@@ -30181,7 +30181,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="97" spans="1:17">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" s="38">
         <v>45964</v>
       </c>
@@ -30227,7 +30227,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="98" spans="1:17">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98" s="38">
         <v>45965</v>
       </c>
@@ -30273,7 +30273,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="99" spans="1:17">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" s="38">
         <v>45966</v>
       </c>
@@ -30319,7 +30319,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="100" spans="1:17">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A100" s="38">
         <v>45967</v>
       </c>
@@ -30365,7 +30365,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="101" spans="1:17">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" s="38">
         <v>45968</v>
       </c>
@@ -30411,7 +30411,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="102" spans="1:17">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" s="38">
         <v>45969</v>
       </c>
@@ -30457,7 +30457,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="103" spans="1:17">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103" s="38">
         <v>45970</v>
       </c>
@@ -30503,7 +30503,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="104" spans="1:17">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104" s="38">
         <v>45971</v>
       </c>
@@ -30549,7 +30549,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="105" spans="1:17">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A105" s="38">
         <v>45972</v>
       </c>
@@ -30595,7 +30595,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="106" spans="1:17">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A106" s="38">
         <v>45973</v>
       </c>
@@ -30641,7 +30641,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="107" spans="1:17">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A107" s="38">
         <v>45974</v>
       </c>
@@ -30687,7 +30687,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="108" spans="1:17">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A108" s="38">
         <v>45975</v>
       </c>
@@ -30733,7 +30733,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="109" spans="1:17">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A109" s="38">
         <v>45976</v>
       </c>
@@ -30779,7 +30779,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="110" spans="1:17">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A110" s="38">
         <v>45977</v>
       </c>
@@ -30825,7 +30825,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="111" spans="1:17">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A111" s="38">
         <v>45978</v>
       </c>
@@ -30871,7 +30871,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="112" spans="1:17">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A112" s="38">
         <v>45979</v>
       </c>
@@ -30917,7 +30917,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="113" spans="1:17">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A113" s="38">
         <v>45980</v>
       </c>
@@ -30963,7 +30963,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="114" spans="1:17">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A114" s="38">
         <v>45981</v>
       </c>
@@ -31009,7 +31009,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="115" spans="1:17">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A115" s="38">
         <v>45982</v>
       </c>
@@ -31055,7 +31055,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="116" spans="1:17">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A116" s="38">
         <v>45983</v>
       </c>
@@ -31101,7 +31101,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="117" spans="1:17">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A117" s="38">
         <v>45984</v>
       </c>
@@ -31147,7 +31147,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="118" spans="1:17">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A118" s="38">
         <v>45985</v>
       </c>
@@ -31193,7 +31193,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="119" spans="1:17">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A119" s="38">
         <v>45986</v>
       </c>
@@ -31239,7 +31239,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="120" spans="1:17">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A120" s="38">
         <v>45987</v>
       </c>
@@ -31285,7 +31285,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="121" spans="1:17">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A121" s="38">
         <v>45988</v>
       </c>
@@ -31331,7 +31331,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="122" spans="1:17">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A122" s="38">
         <v>45989</v>
       </c>
@@ -31377,7 +31377,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="123" spans="1:17">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A123" s="38">
         <v>45990</v>
       </c>
@@ -31423,7 +31423,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="124" spans="1:17">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A124" s="38">
         <v>45991</v>
       </c>
@@ -31469,7 +31469,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="125" spans="1:17">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A125" s="38">
         <v>45992</v>
       </c>
@@ -31515,7 +31515,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="126" spans="1:17">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A126" s="38">
         <v>45993</v>
       </c>
@@ -31561,7 +31561,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="127" spans="1:17">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A127" s="38">
         <v>45994</v>
       </c>
@@ -31607,7 +31607,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="128" spans="1:17">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A128" s="38">
         <v>45995</v>
       </c>
@@ -31653,7 +31653,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="129" spans="1:17">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A129" s="38">
         <v>45996</v>
       </c>
@@ -31699,7 +31699,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="130" spans="1:17">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A130" s="38">
         <v>45997</v>
       </c>
@@ -31745,7 +31745,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="131" spans="1:17">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A131" s="38">
         <v>45998</v>
       </c>
@@ -31791,7 +31791,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="132" spans="1:17">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A132" s="38">
         <v>45999</v>
       </c>
@@ -31837,7 +31837,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="133" spans="1:17">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A133" s="38">
         <v>46000</v>
       </c>
@@ -31883,7 +31883,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="134" spans="1:17">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A134" s="38">
         <v>46001</v>
       </c>
@@ -31929,7 +31929,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="135" spans="1:17">
+    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A135" s="38">
         <v>46002</v>
       </c>
@@ -31975,7 +31975,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="136" spans="1:17">
+    <row r="136" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A136" s="38">
         <v>46003</v>
       </c>
@@ -32021,7 +32021,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="137" spans="1:17">
+    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A137" s="38">
         <v>46004</v>
       </c>
@@ -32067,7 +32067,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="138" spans="1:17">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A138" s="38">
         <v>46005</v>
       </c>
@@ -32113,7 +32113,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="139" spans="1:17">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A139" s="38">
         <v>46006</v>
       </c>
@@ -32159,7 +32159,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="140" spans="1:17">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A140" s="38">
         <v>46007</v>
       </c>
@@ -32205,7 +32205,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="141" spans="1:17">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A141" s="38">
         <v>46008</v>
       </c>
@@ -32251,7 +32251,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="142" spans="1:17">
+    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A142" s="38">
         <v>46009</v>
       </c>
@@ -32297,7 +32297,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="143" spans="1:17">
+    <row r="143" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A143" s="38">
         <v>46010</v>
       </c>
@@ -32343,7 +32343,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="144" spans="1:17">
+    <row r="144" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A144" s="38">
         <v>46011</v>
       </c>
@@ -32389,7 +32389,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="145" spans="1:17">
+    <row r="145" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A145" s="38">
         <v>46012</v>
       </c>
@@ -32435,7 +32435,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="146" spans="1:17">
+    <row r="146" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A146" s="38">
         <v>46013</v>
       </c>
@@ -32481,7 +32481,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="147" spans="1:17">
+    <row r="147" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A147" s="38">
         <v>46014</v>
       </c>
@@ -32527,7 +32527,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="148" spans="1:17">
+    <row r="148" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A148" s="38">
         <v>46015</v>
       </c>
@@ -32573,7 +32573,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="149" spans="1:17">
+    <row r="149" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A149" s="38">
         <v>46016</v>
       </c>
@@ -32619,7 +32619,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="150" spans="1:17">
+    <row r="150" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A150" s="38">
         <v>46017</v>
       </c>
@@ -32665,7 +32665,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="151" spans="1:17">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A151" s="38">
         <v>46018</v>
       </c>
@@ -32711,7 +32711,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="152" spans="1:17">
+    <row r="152" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A152" s="38">
         <v>46019</v>
       </c>
@@ -32757,7 +32757,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="153" spans="1:17">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A153" s="38">
         <v>46020</v>
       </c>
@@ -32803,7 +32803,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="154" spans="1:17">
+    <row r="154" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A154" s="38">
         <v>46021</v>
       </c>
@@ -32849,7 +32849,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="155" spans="1:17">
+    <row r="155" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A155" s="38">
         <v>46022</v>
       </c>
@@ -32895,7 +32895,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="156" spans="1:17">
+    <row r="156" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A156" s="38">
         <v>46023</v>
       </c>
@@ -32941,7 +32941,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="157" spans="1:17">
+    <row r="157" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A157" s="38">
         <v>46024</v>
       </c>
@@ -32987,7 +32987,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="158" spans="1:17">
+    <row r="158" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A158" s="38">
         <v>46025</v>
       </c>
@@ -33033,7 +33033,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="159" spans="1:17">
+    <row r="159" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A159" s="38">
         <v>46026</v>
       </c>
@@ -33079,7 +33079,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="160" spans="1:17">
+    <row r="160" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A160" s="38">
         <v>46027</v>
       </c>
@@ -33125,7 +33125,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="161" spans="1:17">
+    <row r="161" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A161" s="38">
         <v>46028</v>
       </c>
@@ -33171,7 +33171,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="162" spans="1:17">
+    <row r="162" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A162" s="38">
         <v>46029</v>
       </c>
@@ -33217,7 +33217,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="163" spans="1:17">
+    <row r="163" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A163" s="38">
         <v>46030</v>
       </c>
@@ -33263,7 +33263,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="164" spans="1:17">
+    <row r="164" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A164" s="38">
         <v>46031</v>
       </c>
@@ -33309,7 +33309,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="165" spans="1:17">
+    <row r="165" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A165" s="38">
         <v>46032</v>
       </c>
@@ -33355,7 +33355,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="166" spans="1:17">
+    <row r="166" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A166" s="38">
         <v>46033</v>
       </c>
@@ -33401,7 +33401,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="167" spans="1:17">
+    <row r="167" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A167" s="38">
         <v>46034</v>
       </c>
@@ -33447,7 +33447,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="168" spans="1:17">
+    <row r="168" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A168" s="38">
         <v>46035</v>
       </c>
@@ -33493,7 +33493,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="169" spans="1:17">
+    <row r="169" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A169" s="38">
         <v>46036</v>
       </c>
@@ -33539,7 +33539,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="170" spans="1:17">
+    <row r="170" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A170" s="38">
         <v>46037</v>
       </c>
@@ -33585,7 +33585,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="171" spans="1:17">
+    <row r="171" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A171" s="38">
         <v>46038</v>
       </c>
@@ -33631,7 +33631,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="172" spans="1:17">
+    <row r="172" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A172" s="38">
         <v>46039</v>
       </c>
@@ -33677,7 +33677,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="173" spans="1:17">
+    <row r="173" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A173" s="38">
         <v>46040</v>
       </c>
@@ -33723,7 +33723,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="174" spans="1:17">
+    <row r="174" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A174" s="38">
         <v>46041</v>
       </c>
@@ -33769,7 +33769,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="175" spans="1:17">
+    <row r="175" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A175" s="38">
         <v>46042</v>
       </c>
@@ -33815,7 +33815,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="176" spans="1:17">
+    <row r="176" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A176" s="38">
         <v>46043</v>
       </c>
@@ -33861,7 +33861,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="177" spans="1:17">
+    <row r="177" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A177" s="38">
         <v>46044</v>
       </c>
@@ -33907,7 +33907,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="178" spans="1:17">
+    <row r="178" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A178" s="38">
         <v>46045</v>
       </c>
@@ -33953,7 +33953,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="179" spans="1:17">
+    <row r="179" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A179" s="38">
         <v>46046</v>
       </c>
@@ -33999,7 +33999,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="180" spans="1:17">
+    <row r="180" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A180" s="38">
         <v>46047</v>
       </c>
@@ -34045,7 +34045,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="181" spans="1:17">
+    <row r="181" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A181" s="38">
         <v>46048</v>
       </c>
@@ -34091,7 +34091,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="182" spans="1:17">
+    <row r="182" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A182" s="38">
         <v>46049</v>
       </c>
@@ -34137,7 +34137,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="183" spans="1:17">
+    <row r="183" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A183" s="38">
         <v>46050</v>
       </c>
@@ -34183,7 +34183,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="184" spans="1:17">
+    <row r="184" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A184" s="38">
         <v>46051</v>
       </c>
@@ -34229,7 +34229,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="185" spans="1:17">
+    <row r="185" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A185" s="38">
         <v>46052</v>
       </c>
@@ -34275,7 +34275,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="186" spans="1:17">
+    <row r="186" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A186" s="38">
         <v>46053</v>
       </c>
@@ -34321,7 +34321,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="187" spans="1:17">
+    <row r="187" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A187" s="38">
         <v>46054</v>
       </c>
@@ -34367,7 +34367,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="188" spans="1:17">
+    <row r="188" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A188" s="38">
         <v>46055</v>
       </c>
@@ -34413,7 +34413,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="189" spans="1:17">
+    <row r="189" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A189" s="38">
         <v>46056</v>
       </c>
@@ -34459,7 +34459,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="190" spans="1:17">
+    <row r="190" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A190" s="38">
         <v>46057</v>
       </c>
@@ -34505,7 +34505,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="191" spans="1:17">
+    <row r="191" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A191" s="38">
         <v>46058</v>
       </c>
@@ -34551,7 +34551,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="192" spans="1:17">
+    <row r="192" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A192" s="38">
         <v>46059</v>
       </c>
@@ -34597,7 +34597,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="193" spans="1:17">
+    <row r="193" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A193" s="38">
         <v>46060</v>
       </c>
@@ -34643,7 +34643,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="194" spans="1:17">
+    <row r="194" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A194" s="38">
         <v>46061</v>
       </c>
@@ -34689,7 +34689,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="195" spans="1:17">
+    <row r="195" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A195" s="38">
         <v>46062</v>
       </c>
@@ -34735,7 +34735,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="196" spans="1:17">
+    <row r="196" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A196" s="38">
         <v>46063</v>
       </c>
@@ -34781,7 +34781,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="197" spans="1:17">
+    <row r="197" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A197" s="38">
         <v>46064</v>
       </c>
@@ -34827,7 +34827,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="198" spans="1:17">
+    <row r="198" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A198" s="38">
         <v>46065</v>
       </c>
@@ -34873,7 +34873,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="199" spans="1:17">
+    <row r="199" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A199" s="38">
         <v>46066</v>
       </c>
@@ -34919,7 +34919,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="200" spans="1:17">
+    <row r="200" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A200" s="38">
         <v>46067</v>
       </c>
@@ -34965,7 +34965,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="201" spans="1:17">
+    <row r="201" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A201" s="38">
         <v>46068</v>
       </c>
@@ -35011,7 +35011,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="202" spans="1:17">
+    <row r="202" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A202" s="38">
         <v>46069</v>
       </c>
@@ -35057,7 +35057,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="203" spans="1:17">
+    <row r="203" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A203" s="38">
         <v>46070</v>
       </c>
@@ -35103,7 +35103,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="204" spans="1:17">
+    <row r="204" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A204" s="38">
         <v>46071</v>
       </c>
@@ -35149,7 +35149,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="205" spans="1:17">
+    <row r="205" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A205" s="38">
         <v>46072</v>
       </c>
@@ -35195,7 +35195,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="206" spans="1:17">
+    <row r="206" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A206" s="38">
         <v>46073</v>
       </c>
@@ -35241,7 +35241,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="207" spans="1:17">
+    <row r="207" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A207" s="38">
         <v>46074</v>
       </c>
@@ -35287,7 +35287,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="208" spans="1:17">
+    <row r="208" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A208" s="38">
         <v>46075</v>
       </c>
@@ -35333,7 +35333,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="209" spans="1:17">
+    <row r="209" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A209" s="38">
         <v>46076</v>
       </c>
@@ -35379,7 +35379,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="210" spans="1:17">
+    <row r="210" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A210" s="38">
         <v>46077</v>
       </c>
@@ -35425,7 +35425,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="211" spans="1:17">
+    <row r="211" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A211" s="38">
         <v>46078</v>
       </c>
@@ -35471,7 +35471,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="212" spans="1:17">
+    <row r="212" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A212" s="38">
         <v>46079</v>
       </c>
@@ -35517,7 +35517,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="213" spans="1:17">
+    <row r="213" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A213" s="38">
         <v>46080</v>
       </c>
@@ -35563,7 +35563,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="214" spans="1:17">
+    <row r="214" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A214" s="38">
         <v>46081</v>
       </c>
@@ -35609,7 +35609,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="215" spans="1:17">
+    <row r="215" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A215" s="38"/>
       <c r="B215" s="30"/>
       <c r="C215"/>
@@ -35626,7 +35626,7 @@
       <c r="P215" s="20"/>
       <c r="Q215" s="28"/>
     </row>
-    <row r="216" spans="1:17">
+    <row r="216" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A216" s="32"/>
       <c r="B216" s="32"/>
       <c r="C216"/>
@@ -35641,7 +35641,7 @@
       <c r="M216" s="22"/>
       <c r="P216" s="22"/>
     </row>
-    <row r="217" spans="1:17">
+    <row r="217" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A217" s="39" t="s">
         <v>15</v>
       </c>
@@ -35700,7 +35700,7 @@
       </c>
       <c r="P217" s="23"/>
     </row>
-    <row r="218" spans="1:17" s="27" customFormat="1">
+    <row r="218" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A218" s="35" t="s">
         <v>16</v>
       </c>
@@ -35759,7 +35759,7 @@
       </c>
       <c r="P218" s="23"/>
     </row>
-    <row r="219" spans="1:17" s="27" customFormat="1">
+    <row r="219" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A219" s="16" t="s">
         <v>17</v>
       </c>
@@ -35818,7 +35818,7 @@
       </c>
       <c r="P219" s="23"/>
     </row>
-    <row r="220" spans="1:17" s="27" customFormat="1">
+    <row r="220" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A220" s="16" t="s">
         <v>18</v>
       </c>
@@ -35877,7 +35877,7 @@
       </c>
       <c r="P220" s="23"/>
     </row>
-    <row r="221" spans="1:17" s="27" customFormat="1">
+    <row r="221" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A221" s="16" t="s">
         <v>19</v>
       </c>
@@ -35936,7 +35936,7 @@
       </c>
       <c r="P221" s="23"/>
     </row>
-    <row r="222" spans="1:17" s="27" customFormat="1">
+    <row r="222" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A222" s="16" t="s">
         <v>20</v>
       </c>
@@ -35995,7 +35995,7 @@
       </c>
       <c r="P222" s="23"/>
     </row>
-    <row r="223" spans="1:17" s="27" customFormat="1">
+    <row r="223" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A223" s="16" t="s">
         <v>21</v>
       </c>
@@ -36054,7 +36054,7 @@
       </c>
       <c r="P223" s="23"/>
     </row>
-    <row r="224" spans="1:17" s="27" customFormat="1">
+    <row r="224" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A224" s="16" t="s">
         <v>22</v>
       </c>
@@ -36074,7 +36074,7 @@
       <c r="O224" s="23"/>
       <c r="P224" s="23"/>
     </row>
-    <row r="225" spans="1:16" s="27" customFormat="1">
+    <row r="225" spans="1:16" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A225" s="16" t="s">
         <v>23</v>
       </c>
@@ -36133,7 +36133,7 @@
       </c>
       <c r="P225" s="23"/>
     </row>
-    <row r="226" spans="1:16" s="27" customFormat="1">
+    <row r="226" spans="1:16" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A226" s="16" t="s">
         <v>24</v>
       </c>
@@ -36192,7 +36192,7 @@
       </c>
       <c r="P226" s="23"/>
     </row>
-    <row r="227" spans="1:16">
+    <row r="227" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A227" s="16" t="s">
         <v>25</v>
       </c>
@@ -36251,7 +36251,7 @@
       </c>
       <c r="P227" s="23"/>
     </row>
-    <row r="228" spans="1:16">
+    <row r="228" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A228" s="16" t="s">
         <v>26</v>
       </c>
@@ -36310,7 +36310,7 @@
       </c>
       <c r="P228" s="23"/>
     </row>
-    <row r="229" spans="1:16">
+    <row r="229" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A229" s="16" t="s">
         <v>27</v>
       </c>
@@ -36368,7 +36368,7 @@
       </c>
       <c r="P229" s="23"/>
     </row>
-    <row r="230" spans="1:16">
+    <row r="230" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A230" s="16" t="s">
         <v>28</v>
       </c>
@@ -36426,7 +36426,7 @@
       </c>
       <c r="P230" s="23"/>
     </row>
-    <row r="231" spans="1:16">
+    <row r="231" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A231" s="16" t="s">
         <v>29</v>
       </c>
@@ -36484,12 +36484,12 @@
       </c>
       <c r="P231" s="22"/>
     </row>
-    <row r="232" spans="1:16">
+    <row r="232" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C232"/>
       <c r="D232"/>
       <c r="I232" s="22"/>
     </row>
-    <row r="233" spans="1:16">
+    <row r="233" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A233" s="16" t="s">
         <v>30</v>
       </c>
@@ -36502,7 +36502,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="234" spans="1:16">
+    <row r="234" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A234" s="16" t="s">
         <v>31</v>
       </c>
@@ -36515,7 +36515,7 @@
         <v>2505</v>
       </c>
     </row>
-    <row r="235" spans="1:16">
+    <row r="235" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A235" s="16" t="s">
         <v>32</v>
       </c>
@@ -36528,7 +36528,7 @@
         <v>2545</v>
       </c>
     </row>
-    <row r="236" spans="1:16">
+    <row r="236" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A236" s="16" t="s">
         <v>33</v>
       </c>
@@ -36541,7 +36541,7 @@
         <v>2677</v>
       </c>
     </row>
-    <row r="237" spans="1:16">
+    <row r="237" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A237" s="16" t="s">
         <v>34</v>
       </c>
@@ -36554,7 +36554,7 @@
         <v>3035</v>
       </c>
     </row>
-    <row r="238" spans="1:16">
+    <row r="238" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A238" s="16" t="s">
         <v>35</v>
       </c>
@@ -36567,31 +36567,31 @@
         <v>3568</v>
       </c>
     </row>
-    <row r="239" spans="1:16">
+    <row r="239" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C239"/>
       <c r="D239"/>
     </row>
-    <row r="240" spans="1:16">
+    <row r="240" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C240"/>
       <c r="D240"/>
     </row>
-    <row r="241" spans="3:4">
+    <row r="241" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C241"/>
       <c r="D241"/>
     </row>
-    <row r="242" spans="3:4">
+    <row r="242" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C242"/>
       <c r="D242"/>
     </row>
-    <row r="243" spans="3:4">
+    <row r="243" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C243"/>
       <c r="D243"/>
     </row>
-    <row r="244" spans="3:4">
+    <row r="244" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C244"/>
       <c r="D244"/>
     </row>
-    <row r="245" spans="3:4">
+    <row r="245" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C245"/>
       <c r="D245"/>
     </row>
@@ -36609,12 +36609,12 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
         <v>36</v>
       </c>
@@ -36622,7 +36622,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>3</v>
       </c>
@@ -36630,7 +36630,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>4</v>
       </c>
@@ -36638,7 +36638,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>5</v>
       </c>
@@ -36646,7 +36646,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>6</v>
       </c>
@@ -36654,7 +36654,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>7</v>
       </c>
@@ -36662,7 +36662,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>8</v>
       </c>
@@ -36670,7 +36670,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>9</v>
       </c>
@@ -36678,7 +36678,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>10</v>
       </c>
@@ -36686,7 +36686,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>11</v>
       </c>
@@ -36694,7 +36694,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>12</v>
       </c>
@@ -36702,7 +36702,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>13</v>
       </c>
@@ -36710,25 +36710,25 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="19"/>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="58"/>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="19"/>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="19"/>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="19"/>
     </row>
   </sheetData>
@@ -36744,60 +36744,60 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="18.75">
+    <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="47" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="17.850000000000001" customHeight="1">
+    <row r="2" spans="1:1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="43"/>
     </row>
-    <row r="3" spans="1:1" ht="15.75">
+    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="45" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.75">
+    <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="45"/>
     </row>
-    <row r="5" spans="1:1" ht="15.75">
+    <row r="5" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="45" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15.75">
+    <row r="6" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="45"/>
     </row>
-    <row r="7" spans="1:1" ht="15.75">
+    <row r="7" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="45" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="42"/>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="42"/>
     </row>
-    <row r="11" spans="1:1" ht="15.75">
+    <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="44"/>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="42" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="15.75">
+    <row r="13" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="44"/>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="46" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -36816,136 +36816,136 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" style="2" customWidth="1"/>
     <col min="2" max="16384" width="8.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="36">
+    <row r="1" spans="1:2" ht="36" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>49</v>
       </c>
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="1:2" ht="15.75">
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>50</v>
       </c>
       <c r="B4" s="5"/>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>51</v>
       </c>
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:2" ht="15.75">
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>52</v>
       </c>
       <c r="B6" s="5"/>
     </row>
-    <row r="7" spans="1:2" ht="15.75">
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>53</v>
       </c>
       <c r="B7" s="6"/>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>54</v>
       </c>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>55</v>
       </c>
       <c r="B9" s="4"/>
     </row>
-    <row r="10" spans="1:2" ht="15.75">
+    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>56</v>
       </c>
       <c r="B10" s="5"/>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>57</v>
       </c>
       <c r="B11" s="7"/>
     </row>
-    <row r="12" spans="1:2" ht="15.75">
+    <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>58</v>
       </c>
       <c r="B12" s="5"/>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>59</v>
       </c>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:2" ht="15.75">
+    <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>60</v>
       </c>
       <c r="B14" s="5"/>
     </row>
-    <row r="15" spans="1:2" s="24" customFormat="1" ht="15.75">
+    <row r="15" spans="1:2" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>61</v>
       </c>
       <c r="B15" s="6"/>
     </row>
-    <row r="16" spans="1:2" ht="15.75">
+    <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>62</v>
       </c>
       <c r="B16" s="6"/>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>63</v>
       </c>
       <c r="B17" s="4"/>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.75">
+    <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="56"/>
     </row>
-    <row r="21" spans="1:2" ht="15.75">
+    <row r="21" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="57"/>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="15"/>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="17"/>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="37"/>
     </row>
   </sheetData>

</xml_diff>